<commit_message>
added all unique SPZ to pocty prujezdu
</commit_message>
<xml_diff>
--- a/out_poznamky.xlsx
+++ b/out_poznamky.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vladi\Desktop\auta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD499CC9-B85A-41B6-AB88-DA8672E1858F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0E0E03-3FBF-4FC9-93B5-0E3C32CD6527}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="-120" windowWidth="37680" windowHeight="21840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="-120" windowWidth="37680" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Počty vozidel" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="413">
   <si>
     <t>Základní výstupní tabulky (počty všech vozidel)</t>
   </si>
@@ -1251,21 +1251,6 @@
     <t>EN717KW</t>
   </si>
   <si>
-    <t>SEM PŘIDAT KONTROLNÍ SLOUPEC, POČET NAČTENÝCH DAT V KAŽDEM SLOUPCI..</t>
-  </si>
-  <si>
-    <t>Nedává smysl, neboť některé záznamy se tam dost opakujííí</t>
-  </si>
-  <si>
-    <t>1-3-5-12</t>
-  </si>
-  <si>
-    <t>tady jako 3 jízdy</t>
-  </si>
-  <si>
-    <t>ale v reálu jsou to 4 záznamy</t>
-  </si>
-  <si>
     <t>seznam veškerých SPZ</t>
   </si>
   <si>
@@ -1279,15 +1264,6 @@
   </si>
   <si>
     <t>smazat počet SPZ</t>
-  </si>
-  <si>
-    <t>1,3,5</t>
-  </si>
-  <si>
-    <t>SLUPEC</t>
-  </si>
-  <si>
-    <t>5x</t>
   </si>
   <si>
     <t>ověřit přes časové údaje</t>
@@ -1426,17 +1402,21 @@
     <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1448,10 +1428,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1981,10 +1957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA35"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1992,100 +1968,97 @@
     <col min="1" max="23" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-    </row>
-    <row r="2" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+    <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+    </row>
+    <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="12">
+      <c r="C4" s="13">
         <v>1</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13">
         <v>2</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13">
         <v>3</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12">
+      <c r="H4" s="13"/>
+      <c r="I4" s="13">
         <v>4</v>
       </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12">
+      <c r="J4" s="13"/>
+      <c r="K4" s="13">
         <v>5</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12">
+      <c r="L4" s="13"/>
+      <c r="M4" s="13">
         <v>6</v>
       </c>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12">
+      <c r="N4" s="13"/>
+      <c r="O4" s="13">
         <v>7</v>
       </c>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12">
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13">
         <v>8</v>
       </c>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12">
+      <c r="R4" s="13"/>
+      <c r="S4" s="13">
         <v>9</v>
       </c>
-      <c r="T4" s="12"/>
-      <c r="U4" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="T4" s="13"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -2145,8 +2118,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>1</v>
       </c>
       <c r="B6" s="2">
@@ -2206,12 +2179,9 @@
       <c r="T6">
         <v>16</v>
       </c>
-      <c r="Y6" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
       <c r="B7" s="2">
         <v>2</v>
       </c>
@@ -2269,15 +2239,9 @@
       <c r="T7">
         <v>1</v>
       </c>
-      <c r="Y7" t="s">
-        <v>407</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
         <v>2</v>
       </c>
       <c r="B8" s="2">
@@ -2338,8 +2302,8 @@
         <v>823</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
       <c r="B9" s="2">
         <v>4</v>
       </c>
@@ -2398,8 +2362,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
         <v>3</v>
       </c>
       <c r="B10" s="2">
@@ -2460,8 +2424,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
       <c r="B11" s="2">
         <v>6</v>
       </c>
@@ -2520,8 +2484,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
         <v>4</v>
       </c>
       <c r="B12" s="2">
@@ -2581,12 +2545,9 @@
       <c r="T12">
         <v>40</v>
       </c>
-      <c r="X12" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
       <c r="B13" s="2">
         <v>8</v>
       </c>
@@ -2644,12 +2605,9 @@
       <c r="T13">
         <v>6</v>
       </c>
-      <c r="X13">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
         <v>5</v>
       </c>
       <c r="B14" s="2">
@@ -2709,12 +2667,9 @@
       <c r="T14">
         <v>124</v>
       </c>
-      <c r="X14">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
       <c r="B15" s="2">
         <v>10</v>
       </c>
@@ -2772,12 +2727,9 @@
       <c r="T15">
         <v>3</v>
       </c>
-      <c r="X15" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
         <v>6</v>
       </c>
       <c r="B16" s="2">
@@ -2838,8 +2790,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
       <c r="B17" s="2">
         <v>12</v>
       </c>
@@ -2898,8 +2850,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
         <v>7</v>
       </c>
       <c r="B18" s="2">
@@ -2960,8 +2912,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
       <c r="B19" s="2">
         <v>14</v>
       </c>
@@ -3020,8 +2972,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
         <v>8</v>
       </c>
       <c r="B20" s="2">
@@ -3082,8 +3034,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
       <c r="B21" s="2">
         <v>16</v>
       </c>
@@ -3142,8 +3094,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
         <v>9</v>
       </c>
       <c r="B22" s="2">
@@ -3204,8 +3156,8 @@
         <v>276</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
       <c r="B23" s="2">
         <v>18</v>
       </c>
@@ -3264,26 +3216,26 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+    <row r="25" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="12"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="1" t="s">
         <v>8</v>
       </c>
@@ -3311,16 +3263,15 @@
       <c r="K26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="V26">
-        <f>47217*2</f>
-        <v>94434</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+      <c r="M26" s="11" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="12"/>
+      <c r="B27" s="13"/>
       <c r="C27">
         <v>1107</v>
       </c>
@@ -3349,29 +3300,26 @@
         <v>330</v>
       </c>
     </row>
-    <row r="29" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+    <row r="29" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="P29" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="12"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="1" t="s">
         <v>9</v>
       </c>
@@ -3400,11 +3348,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="12"/>
+      <c r="B31" s="13"/>
       <c r="C31">
         <v>1048</v>
       </c>
@@ -3433,13 +3381,18 @@
         <v>705</v>
       </c>
     </row>
-    <row r="35" spans="16:16" x14ac:dyDescent="0.25">
-      <c r="P35" t="s">
-        <v>417</v>
-      </c>
-    </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="Q4:R4"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A31:B31"/>
@@ -3456,16 +3409,6 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="Q4:R4"/>
   </mergeCells>
   <conditionalFormatting sqref="C27:K27">
     <cfRule type="cellIs" dxfId="9" priority="2" operator="greaterThan">
@@ -3483,6 +3426,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3500,94 +3444,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="12">
+      <c r="C4" s="13">
         <v>1</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13">
         <v>2</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13">
         <v>3</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12">
+      <c r="H4" s="13"/>
+      <c r="I4" s="13">
         <v>4</v>
       </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12">
+      <c r="J4" s="13"/>
+      <c r="K4" s="13">
         <v>5</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12">
+      <c r="L4" s="13"/>
+      <c r="M4" s="13">
         <v>6</v>
       </c>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12">
+      <c r="N4" s="13"/>
+      <c r="O4" s="13">
         <v>7</v>
       </c>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12">
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13">
         <v>8</v>
       </c>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12">
+      <c r="R4" s="13"/>
+      <c r="S4" s="13">
         <v>9</v>
       </c>
-      <c r="T4" s="12"/>
+      <c r="T4" s="13"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -3650,7 +3594,7 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="13">
         <v>1</v>
       </c>
       <c r="B6" s="2">
@@ -3712,7 +3656,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="2">
         <v>2</v>
       </c>
@@ -3772,7 +3716,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="13">
         <v>2</v>
       </c>
       <c r="B8" s="2">
@@ -3834,7 +3778,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="2">
         <v>4</v>
       </c>
@@ -3894,7 +3838,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="13">
         <v>3</v>
       </c>
       <c r="B10" s="2">
@@ -3956,7 +3900,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="2">
         <v>6</v>
       </c>
@@ -4016,7 +3960,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="13">
         <v>4</v>
       </c>
       <c r="B12" s="2">
@@ -4078,7 +4022,7 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="2">
         <v>8</v>
       </c>
@@ -4138,7 +4082,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="13">
         <v>5</v>
       </c>
       <c r="B14" s="2">
@@ -4200,7 +4144,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="2">
         <v>10</v>
       </c>
@@ -4260,7 +4204,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="13">
         <v>6</v>
       </c>
       <c r="B16" s="2">
@@ -4322,7 +4266,7 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="2">
         <v>12</v>
       </c>
@@ -4382,7 +4326,7 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+      <c r="A18" s="13">
         <v>7</v>
       </c>
       <c r="B18" s="2">
@@ -4444,7 +4388,7 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="2">
         <v>14</v>
       </c>
@@ -4504,7 +4448,7 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+      <c r="A20" s="13">
         <v>8</v>
       </c>
       <c r="B20" s="2">
@@ -4566,7 +4510,7 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="2">
         <v>16</v>
       </c>
@@ -4626,7 +4570,7 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
+      <c r="A22" s="13">
         <v>9</v>
       </c>
       <c r="B22" s="2">
@@ -4688,7 +4632,7 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="2">
         <v>18</v>
       </c>
@@ -4748,25 +4692,25 @@
       </c>
     </row>
     <row r="25" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="12"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="1" t="s">
         <v>8</v>
       </c>
@@ -4796,10 +4740,10 @@
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="12"/>
+      <c r="B27" s="13"/>
       <c r="C27">
         <v>0</v>
       </c>
@@ -4829,25 +4773,25 @@
       </c>
     </row>
     <row r="29" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="12"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="1" t="s">
         <v>9</v>
       </c>
@@ -4877,10 +4821,10 @@
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="12"/>
+      <c r="B31" s="13"/>
       <c r="C31">
         <v>0</v>
       </c>
@@ -4911,6 +4855,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="Q4:R4"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A31:B31"/>
@@ -4927,16 +4881,6 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="Q4:R4"/>
   </mergeCells>
   <conditionalFormatting sqref="C27:K27">
     <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
@@ -4971,94 +4915,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
+      <c r="S2" s="14"/>
+      <c r="T2" s="14"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
-      <c r="C4" s="12">
+      <c r="C4" s="13">
         <v>1</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12">
+      <c r="D4" s="13"/>
+      <c r="E4" s="13">
         <v>2</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12">
+      <c r="F4" s="13"/>
+      <c r="G4" s="13">
         <v>3</v>
       </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12">
+      <c r="H4" s="13"/>
+      <c r="I4" s="13">
         <v>4</v>
       </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12">
+      <c r="J4" s="13"/>
+      <c r="K4" s="13">
         <v>5</v>
       </c>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12">
+      <c r="L4" s="13"/>
+      <c r="M4" s="13">
         <v>6</v>
       </c>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12">
+      <c r="N4" s="13"/>
+      <c r="O4" s="13">
         <v>7</v>
       </c>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12">
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13">
         <v>8</v>
       </c>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12">
+      <c r="R4" s="13"/>
+      <c r="S4" s="13">
         <v>9</v>
       </c>
-      <c r="T4" s="12"/>
+      <c r="T4" s="13"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
@@ -5121,7 +5065,7 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="13">
         <v>1</v>
       </c>
       <c r="B6" s="2">
@@ -5183,7 +5127,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="2">
         <v>2</v>
       </c>
@@ -5243,7 +5187,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="13">
         <v>2</v>
       </c>
       <c r="B8" s="2">
@@ -5305,7 +5249,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="2">
         <v>4</v>
       </c>
@@ -5365,7 +5309,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="13">
         <v>3</v>
       </c>
       <c r="B10" s="2">
@@ -5427,7 +5371,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="2">
         <v>6</v>
       </c>
@@ -5487,7 +5431,7 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="13">
         <v>4</v>
       </c>
       <c r="B12" s="2">
@@ -5549,7 +5493,7 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="2">
         <v>8</v>
       </c>
@@ -5609,7 +5553,7 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="13">
         <v>5</v>
       </c>
       <c r="B14" s="2">
@@ -5671,7 +5615,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="2">
         <v>10</v>
       </c>
@@ -5731,7 +5675,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="13">
         <v>6</v>
       </c>
       <c r="B16" s="2">
@@ -5793,7 +5737,7 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="12"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="2">
         <v>12</v>
       </c>
@@ -5853,7 +5797,7 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
+      <c r="A18" s="13">
         <v>7</v>
       </c>
       <c r="B18" s="2">
@@ -5915,7 +5859,7 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
+      <c r="A19" s="13"/>
       <c r="B19" s="2">
         <v>14</v>
       </c>
@@ -5975,7 +5919,7 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="12">
+      <c r="A20" s="13">
         <v>8</v>
       </c>
       <c r="B20" s="2">
@@ -6037,7 +5981,7 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="2">
         <v>16</v>
       </c>
@@ -6097,7 +6041,7 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="12">
+      <c r="A22" s="13">
         <v>9</v>
       </c>
       <c r="B22" s="2">
@@ -6159,7 +6103,7 @@
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+      <c r="A23" s="13"/>
       <c r="B23" s="2">
         <v>18</v>
       </c>
@@ -6219,25 +6163,25 @@
       </c>
     </row>
     <row r="25" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="12"/>
+      <c r="B26" s="13"/>
       <c r="C26" s="1" t="s">
         <v>8</v>
       </c>
@@ -6267,10 +6211,10 @@
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B27" s="12"/>
+      <c r="B27" s="13"/>
       <c r="C27">
         <v>0</v>
       </c>
@@ -6300,25 +6244,25 @@
       </c>
     </row>
     <row r="29" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="12"/>
+      <c r="B30" s="13"/>
       <c r="C30" s="1" t="s">
         <v>9</v>
       </c>
@@ -6348,10 +6292,10 @@
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="12"/>
+      <c r="B31" s="13"/>
       <c r="C31">
         <v>0</v>
       </c>
@@ -6382,6 +6326,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:T2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="Q4:R4"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A27:B27"/>
     <mergeCell ref="A31:B31"/>
@@ -6398,16 +6352,6 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A1:T1"/>
-    <mergeCell ref="A2:T2"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="Q4:R4"/>
   </mergeCells>
   <conditionalFormatting sqref="C27:K27">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
@@ -6433,7 +6377,7 @@
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6446,49 +6390,49 @@
       <c r="A1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13" t="s">
+      <c r="I1" s="16"/>
+      <c r="J1" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13" t="s">
+      <c r="K1" s="16"/>
+      <c r="L1" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13" t="s">
+      <c r="M1" s="16"/>
+      <c r="N1" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13" t="s">
+      <c r="O1" s="16"/>
+      <c r="P1" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13" t="s">
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="13"/>
-      <c r="T1" s="14" t="s">
+      <c r="S1" s="16"/>
+      <c r="T1" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="U1" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="V1" s="14" t="s">
+      <c r="V1" s="15" t="s">
         <v>59</v>
       </c>
     </row>
@@ -6550,9 +6494,9 @@
       <c r="S2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
@@ -6755,7 +6699,7 @@
         <v>7</v>
       </c>
       <c r="T5" s="4">
-        <f t="shared" ref="T3:T16" si="2">SUM(B5:S5) * A5</f>
+        <f t="shared" ref="T5:T16" si="2">SUM(B5:S5) * A5</f>
         <v>1662</v>
       </c>
       <c r="U5" s="5">
@@ -7709,37 +7653,40 @@
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
-        <v>404</v>
-      </c>
+      <c r="A21" s="11"/>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J29" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J30" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J31" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J32" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="33" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J33" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="U1:U2"/>
     <mergeCell ref="V1:V2"/>
     <mergeCell ref="L1:M1"/>
@@ -7747,11 +7694,6 @@
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="T1:T2"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:S17">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
@@ -7767,62 +7709,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Y338"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:25" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="W1" s="15" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="W1" s="17" t="s">
         <v>254</v>
       </c>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
     </row>
     <row r="2" spans="1:25" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="18" t="s">
         <v>62</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="17" t="s">
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="L2" s="19" t="s">
-        <v>420</v>
-      </c>
-      <c r="W2" s="16" t="s">
+      <c r="L2" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="W2" s="18" t="s">
         <v>62</v>
       </c>
       <c r="X2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="Y2" s="17" t="s">
+      <c r="Y2" s="19" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="6" t="s">
-        <v>418</v>
-      </c>
-      <c r="C3" s="20" t="s">
-        <v>419</v>
+        <v>410</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>411</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>65</v>
@@ -7833,12 +7775,12 @@
       <c r="F3" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G3" s="17"/>
-      <c r="W3" s="16"/>
+      <c r="G3" s="19"/>
+      <c r="W3" s="18"/>
       <c r="X3" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="Y3" s="17"/>
+      <c r="Y3" s="19"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -12660,7 +12602,7 @@
         <v>2.6</v>
       </c>
       <c r="G164" s="10">
-        <f t="shared" ref="G164:G195" si="8">SUM(D164:F164)</f>
+        <f t="shared" ref="G164:G190" si="8">SUM(D164:F164)</f>
         <v>10.766666666666666</v>
       </c>
       <c r="W164" s="8" t="s">
@@ -15058,7 +15000,7 @@
         <v>11.16666666666667</v>
       </c>
       <c r="Y324" s="10">
-        <f t="shared" ref="Y324:Y387" si="11">SUM(X324:X324)</f>
+        <f t="shared" ref="Y324:Y338" si="11">SUM(X324:X324)</f>
         <v>11.16666666666667</v>
       </c>
     </row>

</xml_diff>